<commit_message>
updated location of these birds
</commit_message>
<xml_diff>
--- a/BirdShit.xlsx
+++ b/BirdShit.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Matthew\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tszyeunglam/GitHub/CPSC_449_Prolog/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14070" windowHeight="11610"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="14860" windowHeight="16080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -563,17 +569,17 @@
   <dimension ref="A1:AJ32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -587,7 +593,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -598,7 +604,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -609,7 +615,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -623,7 +629,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -640,7 +646,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -657,7 +663,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -674,7 +680,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -682,10 +688,10 @@
         <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -696,12 +702,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -742,7 +748,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -783,7 +789,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -824,7 +830,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -865,7 +871,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -906,7 +912,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -947,7 +953,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -988,7 +994,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -996,28 +1002,28 @@
         <v>17</v>
       </c>
       <c r="F20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I20" t="s">
         <v>17</v>
       </c>
       <c r="L20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="X20" t="s">
         <v>18</v>
       </c>
       <c r="AA20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AD20" t="s">
         <v>17</v>
@@ -1026,10 +1032,10 @@
         <v>17</v>
       </c>
       <c r="AJ20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1043,13 +1049,13 @@
         <v>17</v>
       </c>
       <c r="L21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U21" t="s">
         <v>18</v>
@@ -1058,7 +1064,7 @@
         <v>18</v>
       </c>
       <c r="AA21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AD21" t="s">
         <v>18</v>
@@ -1070,12 +1076,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -1092,7 +1098,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1109,7 +1115,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1126,7 +1132,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -1143,7 +1149,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -1160,7 +1166,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -1177,7 +1183,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -1194,24 +1200,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>15</v>
       </c>
       <c r="C31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I31" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L31" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -1222,7 +1228,7 @@
         <v>18</v>
       </c>
       <c r="I32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L32" t="s">
         <v>18</v>

</xml_diff>